<commit_message>
combine_orders implemented into CLI
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/ordering/Completed Orders/Copper Horse Coffee/combined_order.xlsx
+++ b/WorkBot/main/backend/ordering/Completed Orders/Copper Horse Coffee/combined_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\Andrew\Projects\RandomStuff\WorkBot\main\backend\orders\OrderFiles\Copper Horse Coffee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E656AE-E2C4-4E72-B5B9-D30E32DE202B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB825F2-4E1C-4C3D-9554-4BB390B9EDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,9 @@
     <t>Copper Horse - Warhorse 5lb</t>
   </si>
   <si>
+    <t>Copper Horse - Warhorse Blend (12oz)</t>
+  </si>
+  <si>
     <t>Copper Horse - Rumble Pony (12oz)</t>
   </si>
   <si>
@@ -32,9 +35,6 @@
   </si>
   <si>
     <t>Copper Horse - Carriage House Blend (12oz)</t>
-  </si>
-  <si>
-    <t>Copper Horse - Warhorse Blend (12oz)</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -396,7 +396,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>